<commit_message>
courbe td1 et td2
</commit_message>
<xml_diff>
--- a/Front_end.xlsx
+++ b/Front_end.xlsx
@@ -315,32 +315,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -772,11 +774,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="484500160"/>
-        <c:axId val="484498528"/>
+        <c:axId val="146816784"/>
+        <c:axId val="146817872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="484500160"/>
+        <c:axId val="146816784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,7 +821,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484498528"/>
+        <c:crossAx val="146817872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -827,7 +829,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="484498528"/>
+        <c:axId val="146817872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -878,7 +880,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484500160"/>
+        <c:crossAx val="146816784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1489,11 +1491,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="667220576"/>
-        <c:axId val="667214592"/>
+        <c:axId val="312022944"/>
+        <c:axId val="312027296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="667220576"/>
+        <c:axId val="312022944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1522,7 +1524,7 @@
                   <a:rPr lang="fr-FR" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Contraintes moyennes admissibles en membrane</a:t>
+                  <a:t>Contraintes moyennes admissibles en membrane (bidi)</a:t>
                 </a:r>
                 <a:endParaRPr lang="fr-FR" sz="1100" b="1"/>
               </a:p>
@@ -1595,7 +1597,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="667214592"/>
+        <c:crossAx val="312027296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1603,7 +1605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="667214592"/>
+        <c:axId val="312027296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1654,7 +1656,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="667220576"/>
+        <c:crossAx val="312022944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1775,7 +1777,7 @@
                 </a:solidFill>
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Constante pratique fibre: </a:t>
+              <a:t>Constante pratique flexion (uni): </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" sz="1400" b="0" i="0" kern="1200" spc="0" baseline="0">
@@ -1868,7 +1870,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1264166666666667"/>
+          <c:x val="0.13475000000000001"/>
           <c:y val="0.89031552679810644"/>
         </c:manualLayout>
       </c:layout>
@@ -2173,11 +2175,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="667214048"/>
-        <c:axId val="667208608"/>
+        <c:axId val="312032736"/>
+        <c:axId val="312021856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="667214048"/>
+        <c:axId val="312032736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2220,7 +2222,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="667208608"/>
+        <c:crossAx val="312021856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2228,7 +2230,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="667208608"/>
+        <c:axId val="312021856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2279,7 +2281,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="667214048"/>
+        <c:crossAx val="312032736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2409,7 +2411,7 @@
                 </a:solidFill>
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Constante pratique fibre: </a:t>
+              <a:t>Constante pratique flexion (uni): </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" sz="1400" b="0" i="0" kern="1200" spc="0" baseline="0">
@@ -2729,11 +2731,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="481912688"/>
-        <c:axId val="481906704"/>
+        <c:axId val="312034368"/>
+        <c:axId val="312034912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="481912688"/>
+        <c:axId val="312034368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2775,7 +2777,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481906704"/>
+        <c:crossAx val="312034912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2783,7 +2785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="481906704"/>
+        <c:axId val="312034912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2834,7 +2836,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481912688"/>
+        <c:crossAx val="312034368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2964,7 +2966,7 @@
                 </a:solidFill>
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Constante pratique membrane: </a:t>
+              <a:t>Constante pratique membrane (bidi): </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" sz="1400" b="0" i="0" kern="1200" spc="0" baseline="0">
@@ -3362,11 +3364,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="481914864"/>
-        <c:axId val="481908880"/>
+        <c:axId val="312024032"/>
+        <c:axId val="312025120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="481914864"/>
+        <c:axId val="312024032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3409,7 +3411,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481908880"/>
+        <c:crossAx val="312025120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3417,7 +3419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="481908880"/>
+        <c:axId val="312025120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3468,7 +3470,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481914864"/>
+        <c:crossAx val="312024032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3598,7 +3600,7 @@
                 </a:solidFill>
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Constante pratique membrane : </a:t>
+              <a:t>Constante pratique membrane(bidi) : </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" sz="1400" b="0" i="0" kern="1200" spc="0" baseline="0">
@@ -3981,11 +3983,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="667216768"/>
-        <c:axId val="484153232"/>
+        <c:axId val="312031104"/>
+        <c:axId val="312025664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="667216768"/>
+        <c:axId val="312031104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4028,7 +4030,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484153232"/>
+        <c:crossAx val="312025664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4036,7 +4038,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="484153232"/>
+        <c:axId val="312025664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4087,7 +4089,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="667216768"/>
+        <c:crossAx val="312031104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4217,7 +4219,7 @@
                 </a:solidFill>
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Constante pratique fibre: </a:t>
+              <a:t>Constante pratique flexion (bidi): </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" sz="1400" b="0" i="0" kern="1200" spc="0" baseline="0">
@@ -4310,7 +4312,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20150678040244968"/>
+          <c:x val="0.20984011373578304"/>
           <c:y val="0.88753166435748998"/>
         </c:manualLayout>
       </c:layout>
@@ -4552,11 +4554,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="484158672"/>
-        <c:axId val="484152688"/>
+        <c:axId val="312033280"/>
+        <c:axId val="312033824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="484158672"/>
+        <c:axId val="312033280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4598,7 +4600,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484152688"/>
+        <c:crossAx val="312033824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4606,7 +4608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="484152688"/>
+        <c:axId val="312033824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4657,7 +4659,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484158672"/>
+        <c:crossAx val="312033280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4787,7 +4789,7 @@
                 </a:solidFill>
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Constante pratique fibre: </a:t>
+              <a:t>Constante pratique flexion (bidi): </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" sz="1400" b="0" i="0" kern="1200" spc="0" baseline="0">
@@ -5107,11 +5109,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="488693056"/>
-        <c:axId val="488693600"/>
+        <c:axId val="312030560"/>
+        <c:axId val="312036544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="488693056"/>
+        <c:axId val="312030560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5153,7 +5155,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488693600"/>
+        <c:crossAx val="312036544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5161,7 +5163,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="488693600"/>
+        <c:axId val="312036544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5212,7 +5214,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488693056"/>
+        <c:crossAx val="312030560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5700,11 +5702,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="488701760"/>
-        <c:axId val="488701216"/>
+        <c:axId val="42881072"/>
+        <c:axId val="42882160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="488701760"/>
+        <c:axId val="42881072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5747,7 +5749,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488701216"/>
+        <c:crossAx val="42882160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5755,7 +5757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="488701216"/>
+        <c:axId val="42882160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5806,7 +5808,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488701760"/>
+        <c:crossAx val="42881072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6313,11 +6315,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="484495808"/>
-        <c:axId val="484493632"/>
+        <c:axId val="307777104"/>
+        <c:axId val="307785808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="484495808"/>
+        <c:axId val="307777104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6360,7 +6362,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484493632"/>
+        <c:crossAx val="307785808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6368,7 +6370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="484493632"/>
+        <c:axId val="307785808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6419,7 +6421,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484495808"/>
+        <c:crossAx val="307777104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7322,11 +7324,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="481914320"/>
-        <c:axId val="481907248"/>
+        <c:axId val="307778736"/>
+        <c:axId val="307790704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="481914320"/>
+        <c:axId val="307778736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7369,7 +7371,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481907248"/>
+        <c:crossAx val="307790704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7377,7 +7379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="481907248"/>
+        <c:axId val="307790704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7428,7 +7430,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481914320"/>
+        <c:crossAx val="307778736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7918,11 +7920,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="667217856"/>
-        <c:axId val="667218944"/>
+        <c:axId val="307779824"/>
+        <c:axId val="307781456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="667217856"/>
+        <c:axId val="307779824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7965,7 +7967,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="667218944"/>
+        <c:crossAx val="307781456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7973,7 +7975,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="667218944"/>
+        <c:axId val="307781456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8024,7 +8026,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="667217856"/>
+        <c:crossAx val="307779824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8735,11 +8737,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="481905616"/>
-        <c:axId val="481917584"/>
+        <c:axId val="307780368"/>
+        <c:axId val="307784176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="481905616"/>
+        <c:axId val="307780368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8782,7 +8784,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481917584"/>
+        <c:crossAx val="307784176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8790,7 +8792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="481917584"/>
+        <c:axId val="307784176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8841,7 +8843,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481905616"/>
+        <c:crossAx val="307780368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9629,11 +9631,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="667221120"/>
-        <c:axId val="667215680"/>
+        <c:axId val="307787440"/>
+        <c:axId val="307784720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="667221120"/>
+        <c:axId val="307787440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9662,7 +9664,7 @@
                   <a:rPr lang="fr-FR" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Contraintes moyennes admissibles en membrane</a:t>
+                  <a:t>Contraintes moyennes admissibles en membrane (unidirerctionnel)</a:t>
                 </a:r>
                 <a:endParaRPr lang="fr-FR" sz="1100" b="1"/>
               </a:p>
@@ -9735,7 +9737,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="667215680"/>
+        <c:crossAx val="307784720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9743,7 +9745,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="667215680"/>
+        <c:axId val="307784720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9794,7 +9796,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="667221120"/>
+        <c:crossAx val="307787440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9912,7 +9914,7 @@
               <a:rPr lang="fr-FR" sz="1200" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Constante pratique membrane: </a:t>
+              <a:t>Constante pratique membrane (uni): </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" sz="1200" b="0" i="0" baseline="0">
@@ -10283,11 +10285,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="488699584"/>
-        <c:axId val="488689792"/>
+        <c:axId val="307782000"/>
+        <c:axId val="307780912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="488699584"/>
+        <c:axId val="307782000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10330,7 +10332,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488689792"/>
+        <c:crossAx val="307780912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10338,7 +10340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="488689792"/>
+        <c:axId val="307780912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10389,7 +10391,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488699584"/>
+        <c:crossAx val="307782000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10516,7 +10518,7 @@
               <a:rPr lang="fr-FR" sz="1200" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Constante pratique membrane : </a:t>
+              <a:t>Constante pratique membrane (uni) : </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" sz="1200" b="0" i="0" baseline="0">
@@ -10815,11 +10817,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="481902352"/>
-        <c:axId val="481902896"/>
+        <c:axId val="307783632"/>
+        <c:axId val="307790160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="481902352"/>
+        <c:axId val="307783632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10861,7 +10863,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481902896"/>
+        <c:crossAx val="307790160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10869,7 +10871,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="481902896"/>
+        <c:axId val="307790160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10920,7 +10922,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481902352"/>
+        <c:crossAx val="307783632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20106,8 +20108,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>178</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20168,8 +20170,8 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>179</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20484,8 +20486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB44" sqref="AB44"/>
+    <sheetView tabSelected="1" topLeftCell="O104" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X119" sqref="X119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20495,7 +20497,7 @@
     <col min="10" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -20504,60 +20506,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="P1" s="12" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="N1" s="4"/>
+      <c r="P1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
     </row>
     <row r="2" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="N2" s="4"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -20593,19 +20597,20 @@
       <c r="L3" s="1">
         <v>10</v>
       </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -20641,6 +20646,7 @@
       <c r="L4" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -20676,6 +20682,7 @@
       <c r="L5" s="2">
         <v>90</v>
       </c>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -20711,6 +20718,7 @@
       <c r="L6" s="3">
         <v>18841.2137768014</v>
       </c>
+      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -20746,6 +20754,7 @@
       <c r="L7" s="3">
         <v>18841.2137768014</v>
       </c>
+      <c r="N7" s="4"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -20781,6 +20790,7 @@
       <c r="L8" s="3">
         <v>2382.5687329939001</v>
       </c>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -20816,6 +20826,7 @@
       <c r="L9" s="3">
         <v>0.17812098407912499</v>
       </c>
+      <c r="N9" s="4"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -20851,6 +20862,7 @@
       <c r="L10" s="3">
         <v>-3.3994354322034401E-16</v>
       </c>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -20886,6 +20898,7 @@
       <c r="L11" s="3">
         <v>3.3994354322034401E-16</v>
       </c>
+      <c r="N11" s="4"/>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -20921,6 +20934,7 @@
       <c r="L12" s="3">
         <v>650</v>
       </c>
+      <c r="N12" s="4"/>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -20956,6 +20970,7 @@
       <c r="L13" s="3">
         <v>-650</v>
       </c>
+      <c r="N13" s="4"/>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -20991,6 +21006,7 @@
       <c r="L14" s="3">
         <v>650</v>
       </c>
+      <c r="N14" s="4"/>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -21026,6 +21042,7 @@
       <c r="L15" s="3">
         <v>-650</v>
       </c>
+      <c r="N15" s="4"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -21061,6 +21078,7 @@
       <c r="L16" s="3">
         <v>50</v>
       </c>
+      <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -21096,6 +21114,7 @@
       <c r="L17" s="3">
         <v>-50</v>
       </c>
+      <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -21131,6 +21150,7 @@
       <c r="L18" s="3">
         <v>650</v>
       </c>
+      <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -21166,15 +21186,21 @@
       <c r="L19" s="3">
         <v>-650</v>
       </c>
+      <c r="N19" s="4"/>
     </row>
-    <row r="21" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="N22" s="7"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
+      <c r="N23" s="7"/>
       <c r="P23" s="1" t="s">
         <v>1</v>
       </c>
@@ -21192,7 +21218,8 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
+      <c r="N24" s="7"/>
       <c r="P24" s="1" t="s">
         <v>22</v>
       </c>
@@ -21210,7 +21237,8 @@
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
+      <c r="N25" s="7"/>
       <c r="P25" s="1" t="s">
         <v>23</v>
       </c>
@@ -21228,7 +21256,8 @@
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="10"/>
+      <c r="N26" s="7"/>
       <c r="P26" s="1" t="s">
         <v>24</v>
       </c>
@@ -21246,7 +21275,8 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="10"/>
+      <c r="N27" s="7"/>
       <c r="P27" s="1" t="s">
         <v>25</v>
       </c>
@@ -21264,7 +21294,8 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="10"/>
+      <c r="N28" s="7"/>
       <c r="P28" s="1" t="s">
         <v>26</v>
       </c>
@@ -21282,7 +21313,8 @@
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="10"/>
+      <c r="N29" s="7"/>
       <c r="P29" s="1" t="s">
         <v>27</v>
       </c>
@@ -21300,7 +21332,8 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="10"/>
+      <c r="N30" s="7"/>
       <c r="P30" s="1" t="s">
         <v>28</v>
       </c>
@@ -21318,7 +21351,8 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+      <c r="A31" s="10"/>
+      <c r="N31" s="7"/>
       <c r="P31" s="1" t="s">
         <v>29</v>
       </c>
@@ -21336,7 +21370,8 @@
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+      <c r="A32" s="10"/>
+      <c r="N32" s="7"/>
       <c r="P32" s="1" t="s">
         <v>30</v>
       </c>
@@ -21354,7 +21389,8 @@
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="A33" s="10"/>
+      <c r="N33" s="7"/>
       <c r="P33" s="1" t="s">
         <v>31</v>
       </c>
@@ -21372,7 +21408,8 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
+      <c r="A34" s="10"/>
+      <c r="N34" s="7"/>
       <c r="P34" s="1" t="s">
         <v>32</v>
       </c>
@@ -21390,7 +21427,8 @@
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
+      <c r="A35" s="10"/>
+      <c r="N35" s="7"/>
       <c r="P35" s="1" t="s">
         <v>33</v>
       </c>
@@ -21408,7 +21446,8 @@
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
+      <c r="A36" s="10"/>
+      <c r="N36" s="7"/>
       <c r="P36" s="1" t="s">
         <v>34</v>
       </c>
@@ -21426,7 +21465,8 @@
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
+      <c r="A37" s="10"/>
+      <c r="N37" s="7"/>
       <c r="P37" s="1" t="s">
         <v>35</v>
       </c>
@@ -21444,7 +21484,8 @@
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
+      <c r="A38" s="10"/>
+      <c r="N38" s="7"/>
       <c r="P38" s="1" t="s">
         <v>36</v>
       </c>
@@ -21462,7 +21503,8 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
+      <c r="A39" s="10"/>
+      <c r="N39" s="7"/>
       <c r="P39" s="1" t="s">
         <v>37</v>
       </c>
@@ -21480,7 +21522,8 @@
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
+      <c r="A40" s="10"/>
+      <c r="N40" s="7"/>
       <c r="P40" s="1" t="s">
         <v>38</v>
       </c>
@@ -21498,7 +21541,8 @@
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
+      <c r="A41" s="10"/>
+      <c r="N41" s="7"/>
       <c r="P41" s="1" t="s">
         <v>39</v>
       </c>
@@ -21516,7 +21560,8 @@
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
+      <c r="A42" s="10"/>
+      <c r="N42" s="7"/>
       <c r="P42" s="1" t="s">
         <v>40</v>
       </c>
@@ -21534,7 +21579,8 @@
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="A43" s="10"/>
+      <c r="N43" s="7"/>
       <c r="P43" s="1" t="s">
         <v>41</v>
       </c>
@@ -21552,7 +21598,8 @@
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
+      <c r="A44" s="10"/>
+      <c r="N44" s="7"/>
       <c r="P44" s="1" t="s">
         <v>42</v>
       </c>
@@ -21570,185 +21617,241 @@
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
+      <c r="A45" s="10"/>
+      <c r="N45" s="7"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
+      <c r="A46" s="10"/>
+      <c r="N46" s="7"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
+      <c r="A47" s="10"/>
+      <c r="N47" s="7"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
+      <c r="A48" s="10"/>
+      <c r="N48" s="7"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="N49" s="7"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="N50" s="7"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="N51" s="7"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="N52" s="7"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="N53" s="7"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="N54" s="7"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="N55" s="7"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="N56" s="7"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="9"/>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="N57" s="7"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="N58" s="7"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="9"/>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="10"/>
+      <c r="N59" s="7"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="9"/>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+      <c r="N60" s="7"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="9"/>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="10"/>
+      <c r="N61" s="7"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="9"/>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+      <c r="N62" s="7"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="9"/>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="N63" s="7"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="9"/>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="N64" s="7"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="9"/>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" s="10"/>
+      <c r="N65" s="7"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+      <c r="N66" s="7"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="9"/>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
+      <c r="N67" s="7"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="9"/>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" s="10"/>
+      <c r="N68" s="7"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="9"/>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" s="10"/>
+      <c r="N69" s="7"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="9"/>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" s="10"/>
+      <c r="N70" s="7"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="9"/>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="10"/>
+      <c r="N71" s="7"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="9"/>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" s="10"/>
+      <c r="N72" s="7"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="9"/>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="N73" s="7"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" s="10"/>
+      <c r="N74" s="7"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="9"/>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" s="10"/>
+      <c r="N75" s="7"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="9"/>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" s="10"/>
+      <c r="N76" s="7"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="9"/>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" s="10"/>
+      <c r="N77" s="7"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="9"/>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" s="10"/>
+      <c r="N78" s="7"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="9"/>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" s="10"/>
+      <c r="N79" s="7"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="9"/>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A80" s="10"/>
+      <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="9"/>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81" s="10"/>
+      <c r="N81" s="7"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="9"/>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" s="10"/>
+      <c r="N82" s="7"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="9"/>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A83" s="10"/>
+      <c r="N83" s="7"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A84" s="10"/>
+      <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="9"/>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A85" s="10"/>
+      <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A86" s="10"/>
+      <c r="N86" s="7"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="9"/>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A87" s="10"/>
+      <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="9"/>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A88" s="10"/>
+      <c r="N88" s="7"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A89" s="10"/>
+      <c r="N89" s="7"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A90" s="10"/>
+      <c r="N90" s="7"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="9"/>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" s="10"/>
+      <c r="N91" s="7"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92" s="10"/>
+      <c r="N92" s="7"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="9"/>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A93" s="10"/>
+      <c r="N93" s="7"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="9"/>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A94" s="10"/>
+      <c r="N94" s="7"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="9"/>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A95" s="10"/>
+      <c r="N95" s="7"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="9"/>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A96" s="10"/>
+      <c r="N96" s="7"/>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A97" s="9"/>
+      <c r="A97" s="10"/>
+      <c r="N97" s="7"/>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A98" s="9"/>
+      <c r="A98" s="10"/>
+      <c r="N98" s="7"/>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A99" s="9"/>
+      <c r="A99" s="10"/>
+      <c r="N99" s="7"/>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A100" s="9"/>
+      <c r="A100" s="10"/>
+      <c r="N100" s="7"/>
     </row>
-    <row r="101" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="103" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="s">
+      <c r="A103" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A104" s="10"/>
+      <c r="A104" s="11"/>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A105" s="10"/>
+      <c r="A105" s="11"/>
       <c r="P105" s="1" t="s">
         <v>1</v>
       </c>
@@ -21766,7 +21869,7 @@
       </c>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A106" s="10"/>
+      <c r="A106" s="11"/>
       <c r="P106" s="1" t="s">
         <v>22</v>
       </c>
@@ -21784,7 +21887,7 @@
       </c>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A107" s="10"/>
+      <c r="A107" s="11"/>
       <c r="P107" s="1" t="s">
         <v>23</v>
       </c>
@@ -21802,7 +21905,7 @@
       </c>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A108" s="10"/>
+      <c r="A108" s="11"/>
       <c r="P108" s="1" t="s">
         <v>24</v>
       </c>
@@ -21820,7 +21923,7 @@
       </c>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A109" s="10"/>
+      <c r="A109" s="11"/>
       <c r="P109" s="1" t="s">
         <v>25</v>
       </c>
@@ -21838,7 +21941,7 @@
       </c>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A110" s="10"/>
+      <c r="A110" s="11"/>
       <c r="P110" s="1" t="s">
         <v>26</v>
       </c>
@@ -21856,7 +21959,7 @@
       </c>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A111" s="10"/>
+      <c r="A111" s="11"/>
       <c r="P111" s="1" t="s">
         <v>27</v>
       </c>
@@ -21874,7 +21977,7 @@
       </c>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A112" s="10"/>
+      <c r="A112" s="11"/>
       <c r="P112" s="1" t="s">
         <v>28</v>
       </c>
@@ -21892,7 +21995,7 @@
       </c>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A113" s="10"/>
+      <c r="A113" s="11"/>
       <c r="P113" s="1" t="s">
         <v>29</v>
       </c>
@@ -21910,7 +22013,7 @@
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A114" s="10"/>
+      <c r="A114" s="11"/>
       <c r="P114" s="1" t="s">
         <v>30</v>
       </c>
@@ -21928,7 +22031,7 @@
       </c>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A115" s="10"/>
+      <c r="A115" s="11"/>
       <c r="P115" s="1" t="s">
         <v>31</v>
       </c>
@@ -21946,7 +22049,7 @@
       </c>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A116" s="10"/>
+      <c r="A116" s="11"/>
       <c r="P116" s="1" t="s">
         <v>32</v>
       </c>
@@ -21964,7 +22067,7 @@
       </c>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A117" s="10"/>
+      <c r="A117" s="11"/>
       <c r="P117" s="1" t="s">
         <v>33</v>
       </c>
@@ -21982,7 +22085,7 @@
       </c>
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A118" s="10"/>
+      <c r="A118" s="11"/>
       <c r="P118" s="1" t="s">
         <v>34</v>
       </c>
@@ -22000,7 +22103,7 @@
       </c>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A119" s="10"/>
+      <c r="A119" s="11"/>
       <c r="P119" s="1" t="s">
         <v>35</v>
       </c>
@@ -22018,7 +22121,7 @@
       </c>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A120" s="10"/>
+      <c r="A120" s="11"/>
       <c r="P120" s="1" t="s">
         <v>36</v>
       </c>
@@ -22036,7 +22139,7 @@
       </c>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A121" s="10"/>
+      <c r="A121" s="11"/>
       <c r="P121" s="1" t="s">
         <v>37</v>
       </c>
@@ -22054,7 +22157,7 @@
       </c>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A122" s="10"/>
+      <c r="A122" s="11"/>
       <c r="P122" s="1" t="s">
         <v>38</v>
       </c>
@@ -22072,7 +22175,7 @@
       </c>
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A123" s="10"/>
+      <c r="A123" s="11"/>
       <c r="P123" s="1" t="s">
         <v>39</v>
       </c>
@@ -22090,7 +22193,7 @@
       </c>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A124" s="10"/>
+      <c r="A124" s="11"/>
       <c r="P124" s="1" t="s">
         <v>40</v>
       </c>
@@ -22108,7 +22211,7 @@
       </c>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A125" s="10"/>
+      <c r="A125" s="11"/>
       <c r="P125" s="1" t="s">
         <v>41</v>
       </c>
@@ -22126,7 +22229,7 @@
       </c>
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A126" s="10"/>
+      <c r="A126" s="11"/>
       <c r="P126" s="1" t="s">
         <v>42</v>
       </c>
@@ -22144,226 +22247,226 @@
       </c>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A127" s="10"/>
+      <c r="A127" s="11"/>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A128" s="10"/>
+      <c r="A128" s="11"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="10"/>
+      <c r="A129" s="11"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="10"/>
+      <c r="A130" s="11"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="10"/>
+      <c r="A131" s="11"/>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="10"/>
+      <c r="A132" s="11"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="10"/>
+      <c r="A133" s="11"/>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="10"/>
+      <c r="A134" s="11"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="10"/>
+      <c r="A135" s="11"/>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="10"/>
+      <c r="A136" s="11"/>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="10"/>
+      <c r="A137" s="11"/>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="10"/>
+      <c r="A138" s="11"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="10"/>
+      <c r="A139" s="11"/>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="10"/>
+      <c r="A140" s="11"/>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="10"/>
+      <c r="A141" s="11"/>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="10"/>
+      <c r="A142" s="11"/>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="10"/>
+      <c r="A143" s="11"/>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="10"/>
+      <c r="A144" s="11"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="10"/>
+      <c r="A145" s="11"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="10"/>
+      <c r="A146" s="11"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="10"/>
+      <c r="A147" s="11"/>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="10"/>
+      <c r="A148" s="11"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="10"/>
+      <c r="A149" s="11"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="10"/>
+      <c r="A150" s="11"/>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="10"/>
+      <c r="A151" s="11"/>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="10"/>
+      <c r="A152" s="11"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="10"/>
+      <c r="A153" s="11"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="10"/>
+      <c r="A154" s="11"/>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="10"/>
+      <c r="A155" s="11"/>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="10"/>
+      <c r="A156" s="11"/>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="10"/>
+      <c r="A157" s="11"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="10"/>
+      <c r="A158" s="11"/>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="10"/>
+      <c r="A159" s="11"/>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="10"/>
+      <c r="A160" s="11"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="10"/>
+      <c r="A161" s="11"/>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="10"/>
+      <c r="A162" s="11"/>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="10"/>
+      <c r="A163" s="11"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="10"/>
+      <c r="A164" s="11"/>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="10"/>
+      <c r="A165" s="11"/>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="10"/>
+      <c r="A166" s="11"/>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="10"/>
+      <c r="A167" s="11"/>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="10"/>
+      <c r="A168" s="11"/>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="10"/>
+      <c r="A169" s="11"/>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="10"/>
+      <c r="A170" s="11"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="10"/>
+      <c r="A171" s="11"/>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="10"/>
+      <c r="A172" s="11"/>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="10"/>
+      <c r="A173" s="11"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="10"/>
+      <c r="A174" s="11"/>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="10"/>
+      <c r="A175" s="11"/>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="10"/>
+      <c r="A176" s="11"/>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="10"/>
+      <c r="A177" s="11"/>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="10"/>
+      <c r="A178" s="11"/>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="10"/>
+      <c r="A179" s="11"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="10"/>
+      <c r="A180" s="11"/>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="10"/>
+      <c r="A181" s="11"/>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="10"/>
+      <c r="A182" s="11"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="10"/>
+      <c r="A183" s="11"/>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="10"/>
+      <c r="A184" s="11"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="10"/>
+      <c r="A185" s="11"/>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="10"/>
+      <c r="A186" s="11"/>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="10"/>
+      <c r="A187" s="11"/>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="10"/>
+      <c r="A188" s="11"/>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="10"/>
+      <c r="A189" s="11"/>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="10"/>
+      <c r="A190" s="11"/>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="10"/>
+      <c r="A191" s="11"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="10"/>
+      <c r="A192" s="11"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="10"/>
+      <c r="A193" s="11"/>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="10"/>
+      <c r="A194" s="11"/>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="10"/>
+      <c r="A195" s="11"/>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="10"/>
+      <c r="A196" s="11"/>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="10"/>
+      <c r="A197" s="11"/>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="10"/>
+      <c r="A198" s="11"/>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="10"/>
+      <c r="A199" s="11"/>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="10"/>
+      <c r="A200" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>